<commit_message>
New microstates added to SM18 and SM20 (v1.6.1).
</commit_message>
<xml_diff>
--- a/physical_properties/pKa/microstates/SM18_microstate_IDs_with_2D_depiction.xlsx
+++ b/physical_properties/pKa/microstates/SM18_microstate_IDs_with_2D_depiction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="145">
   <si>
     <t>Microstate List</t>
   </si>
@@ -440,6 +440,15 @@
   </si>
   <si>
     <t>c1ccc2c(c1)c(=[OH+])[nH]c(n2)CCC(=O)Nc3ncc(s3)Cc4ccc(c(c4)F)F</t>
+  </si>
+  <si>
+    <t>SM18_micro075</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)c(nc(n2)C/C=C(/N=c/3\[nH]cc(s3)Cc4ccc(c(c4)F)F)\[O-])O</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)c(nc(n2)CC=C(N=c3[nH]cc(s3)Cc4ccc(c(c4)F)F)[O-])O</t>
   </si>
 </sst>
 </file>
@@ -2474,6 +2483,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="158972250"/>
+          <a:ext cx="3175163" cy="3175163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3175163</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>3338</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52" descr="tmp53.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="162144075"/>
           <a:ext cx="3175163" cy="3175163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2771,7 +2818,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3363,6 +3410,17 @@
         <v>141</v>
       </c>
     </row>
+    <row r="54" spans="2:4" s="3" customFormat="1" ht="250.0" customHeight="1">
+      <c r="B54" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
Add microstate ID SM18_micro076 for v1.6.1.
</commit_message>
<xml_diff>
--- a/physical_properties/pKa/microstates/SM18_microstate_IDs_with_2D_depiction.xlsx
+++ b/physical_properties/pKa/microstates/SM18_microstate_IDs_with_2D_depiction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="147">
   <si>
     <t>Microstate List</t>
   </si>
@@ -449,6 +449,12 @@
   </si>
   <si>
     <t>c1ccc2c(c1)c(nc(n2)CC=C(N=c3[nH]cc(s3)Cc4ccc(c(c4)F)F)[O-])O</t>
+  </si>
+  <si>
+    <t>SM18_micro076</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)c(=[OH+])nc([nH]2)CCC(=O)Nc3[nH+]cc(s3)Cc4ccc(c(c4)F)F</t>
   </si>
 </sst>
 </file>
@@ -2521,6 +2527,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="162144075"/>
+          <a:ext cx="3175163" cy="3175163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3175163</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>3338</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53" descr="tmp54.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="165315900"/>
           <a:ext cx="3175163" cy="3175163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2818,7 +2862,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3421,6 +3465,17 @@
         <v>144</v>
       </c>
     </row>
+    <row r="55" spans="2:4" s="2" customFormat="1" ht="250.0" customHeight="1">
+      <c r="B55" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>